<commit_message>
refactor code and unnecessary file remove
</commit_message>
<xml_diff>
--- a/src/main/resources/objectLocator/sample.xlsx
+++ b/src/main/resources/objectLocator/sample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\temp\seleniumAmtTesting\src\main\resources\objectLocator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{846D9494-CC0D-4639-9C90-2D196A926281}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88A64A3C-E4A4-461E-8D23-1292AAD049F7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6945" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
     <t>ObjReference</t>
   </si>
@@ -34,9 +34,6 @@
     <t>by_id</t>
   </si>
   <si>
-    <t>txtUSER_NAME</t>
-  </si>
-  <si>
     <t>password</t>
   </si>
   <si>
@@ -46,19 +43,19 @@
     <t>loginButton</t>
   </si>
   <si>
-    <t>by_xpath</t>
-  </si>
-  <si>
-    <t>//*[@class='btn btn-primary']</t>
-  </si>
-  <si>
     <t>client</t>
   </si>
   <si>
-    <t>txtClient_Number</t>
-  </si>
-  <si>
     <t>ObjectLocators</t>
+  </si>
+  <si>
+    <t>txtUsername</t>
+  </si>
+  <si>
+    <t>btnLogin</t>
+  </si>
+  <si>
+    <t>by_</t>
   </si>
 </sst>
 </file>
@@ -433,7 +430,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -450,7 +447,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -461,40 +458,40 @@
         <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>